<commit_message>
writing script to calc dbpt feats-continuation
</commit_message>
<xml_diff>
--- a/tests/data/test.xlsx
+++ b/tests/data/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ernesto/PycharmProjects/FOREX/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984EDB3A-EDCF-9944-A282-814DB42462DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5FAC67-937C-EE47-BFCC-EDF4DB990697}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>outcome</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>SR</t>
+  </si>
+  <si>
+    <t>short</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -309,7 +312,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -635,9 +638,12 @@
         <v>48</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="AA1" s="1"/>
@@ -667,7 +673,9 @@
       <c r="H2">
         <v>1.84185</v>
       </c>
-      <c r="I2"/>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
       <c r="AA2" s="3"/>
     </row>
     <row r="5" spans="1:27">

</xml_diff>